<commit_message>
added a image to the write up
</commit_message>
<xml_diff>
--- a/write up/Book1.xlsx
+++ b/write up/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfort\Desktop\CPAN-213 0ND\NavigationApp\write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{415AA98C-7F4E-4988-9CC2-15CE060156BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1164F292-9E2E-4DD0-89B4-927673D1211D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{965737AE-01E4-4CE8-B4D0-883CB33A8FF3}"/>
   </bookViews>
@@ -1287,7 +1287,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>

</xml_diff>